<commit_message>
Added memchr, memcmp, strdup. memmove doesnt work and fixed atoi by adding static to the function.
</commit_message>
<xml_diff>
--- a/excel sheet.xlsx
+++ b/excel sheet.xlsx
@@ -217,13 +217,14 @@
     <xf fontId="4" fillId="5" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="6" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="5" borderId="0" numFmtId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="6" borderId="1" numFmtId="0" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,37 +778,37 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -887,12 +888,12 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -909,7 +910,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483647" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
strcat, strncat, strlcat doesn't work fine yet.
</commit_message>
<xml_diff>
--- a/excel sheet.xlsx
+++ b/excel sheet.xlsx
@@ -736,7 +736,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -822,12 +822,12 @@
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>